<commit_message>
feat: adding excels for gpt-5 results
</commit_message>
<xml_diff>
--- a/Results/gpt-5/Chaves2021, 34212033/gpt_answers_60.xlsx
+++ b/Results/gpt-5/Chaves2021, 34212033/gpt_answers_60.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -500,7 +500,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -564,7 +564,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -574,7 +574,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Does the paper report in vitro antiretroviral susceptibility data?</t>
+          <t>Does the paper report novel in vitro antiretroviral susceptibility data?</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -596,7 +596,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -660,7 +660,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -692,7 +692,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -756,7 +756,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -788,7 +788,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -852,7 +852,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -884,7 +884,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -948,7 +948,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -980,7 +980,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1044,7 +1044,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1076,7 +1076,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1140,7 +1140,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1172,7 +1172,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1236,7 +1236,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1268,7 +1268,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1300,7 +1300,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1332,7 +1332,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1364,7 +1364,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1396,7 +1396,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1428,7 +1428,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1460,7 +1460,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1524,7 +1524,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1556,7 +1556,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1620,7 +1620,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1652,7 +1652,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1684,7 +1684,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1716,7 +1716,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1748,7 +1748,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1780,7 +1780,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1812,7 +1812,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1844,7 +1844,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1876,7 +1876,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1908,7 +1908,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1940,7 +1940,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1972,7 +1972,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2004,7 +2004,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2036,7 +2036,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2068,7 +2068,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2100,7 +2100,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2132,7 +2132,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2164,7 +2164,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Does the paper report IC values like IC50? IC90?</t>
+          <t>Does the paper report novel IC values like IC50? IC90?</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -2196,7 +2196,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Does the paper report IC50 fold change values?</t>
+          <t>Does the paper report novel IC50 fold change values?</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2260,7 +2260,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2292,7 +2292,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2324,7 +2324,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2356,7 +2356,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Got2021, 34835480</t>
+          <t>Miti2020, 32804970</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">

</xml_diff>